<commit_message>
put query code into helper functions (streamline code) and ran code to get a few days of data
</commit_message>
<xml_diff>
--- a/data/language-crosswalk.xlsx
+++ b/data/language-crosswalk.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben-tanen/Google Drive/Projects/yt-captions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAC289B6-883D-BD47-A180-75BA8FE511F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97E610C-22E5-EB46-B242-F51AB134C19A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="460" windowWidth="24160" windowHeight="17540" xr2:uid="{6B0037AA-4187-0E48-B1EA-8255E9AAEF56}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{6B0037AA-4187-0E48-B1EA-8255E9AAEF56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$46</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>language</t>
   </si>
@@ -151,13 +154,163 @@
   </si>
   <si>
     <t>Ukrainian</t>
+  </si>
+  <si>
+    <t>en-US</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>de-DE</t>
+  </si>
+  <si>
+    <t>es-ES</t>
+  </si>
+  <si>
+    <t>es-MX</t>
+  </si>
+  <si>
+    <t>fr-FR</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
+  </si>
+  <si>
+    <t>zh-Hans</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>en-CA</t>
+  </si>
+  <si>
+    <t>fa-IR</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>nl-NL</t>
+  </si>
+  <si>
+    <t>zh-Hant</t>
+  </si>
+  <si>
+    <t>pt-PT</t>
+  </si>
+  <si>
+    <t>sv</t>
+  </si>
+  <si>
+    <t>en-GB</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>yue-HK</t>
+  </si>
+  <si>
+    <t>zh-SG</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>zh-HK</t>
+  </si>
+  <si>
+    <t>English (United States)</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>German (Germany)</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>English (Canada)</t>
+  </si>
+  <si>
+    <t>English (United Kingdom)</t>
+  </si>
+  <si>
+    <t>Spanish (Spain)</t>
+  </si>
+  <si>
+    <t>Spanish (Mexico)</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>French (France)</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>Dutch (Netherands)</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Portugese (Portugal)</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Chinese (Hong Kong)</t>
+  </si>
+  <si>
+    <t>Cantonese (Hong Kong)</t>
+  </si>
+  <si>
+    <t>Persian (Iran)</t>
+  </si>
+  <si>
+    <t>Malay</t>
+  </si>
+  <si>
+    <t>Chinese (China)</t>
+  </si>
+  <si>
+    <t>Chinese (Simplified)</t>
+  </si>
+  <si>
+    <t>Chinese (Traditional)</t>
+  </si>
+  <si>
+    <t>Chinese (Singapore)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +325,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,9 +360,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,11 +679,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76702F4A-6822-104D-A228-EE608917D6A9}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -539,158 +705,374 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>37</v>
+      <c r="A5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
+      <c r="A13" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
+      <c r="A14" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
+      <c r="A15" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="A16" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
+      <c r="A18" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
+      <c r="A19" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B46" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:B46" xr:uid="{309F8E5E-ED38-B949-88CE-AFA268C169D7}"/>
+  <sortState ref="A2:B46">
+    <sortCondition ref="A2:A46"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(1) lots of new data, (2) cleaned analysis file
</commit_message>
<xml_diff>
--- a/data/language-crosswalk.xlsx
+++ b/data/language-crosswalk.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben-tanen/Google Drive/Projects/yt-captions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97E610C-22E5-EB46-B242-F51AB134C19A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F17A0D-977E-5C49-BF21-1A11CF53DCC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{6B0037AA-4187-0E48-B1EA-8255E9AAEF56}"/>
+    <workbookView xWindow="13920" yWindow="460" windowWidth="13900" windowHeight="16580" xr2:uid="{6B0037AA-4187-0E48-B1EA-8255E9AAEF56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$55</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>language</t>
   </si>
@@ -304,6 +304,204 @@
   </si>
   <si>
     <t>Chinese (Singapore)</t>
+  </si>
+  <si>
+    <t>en-IE</t>
+  </si>
+  <si>
+    <t>az</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>bn</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>eu</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>fil</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>hu</t>
+  </si>
+  <si>
+    <t>iw</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>mk</t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>sk</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>Azerbaijani</t>
+  </si>
+  <si>
+    <t>Bulgarian</t>
+  </si>
+  <si>
+    <t>Catalan</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Croatian</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>Serbian</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>English (Ireland)</t>
+  </si>
+  <si>
+    <t>Filipino</t>
+  </si>
+  <si>
+    <t>Basque</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
+    <t>Khmer</t>
+  </si>
+  <si>
+    <t>Lao</t>
+  </si>
+  <si>
+    <t>Macedonian</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Slovenian</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Bangla</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>zh</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>hy</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Amhric</t>
+  </si>
+  <si>
+    <t>Amenian</t>
+  </si>
+  <si>
+    <t>Icelandic</t>
+  </si>
+  <si>
+    <t>ru-Latn</t>
+  </si>
+  <si>
+    <t>Russian (Latin)</t>
+  </si>
+  <si>
+    <t>en-IN</t>
+  </si>
+  <si>
+    <t>English (India)</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>Afrikaans</t>
+  </si>
+  <si>
+    <t>fr-CA</t>
+  </si>
+  <si>
+    <t>French (Canada)</t>
+  </si>
+  <si>
+    <t>es-US</t>
+  </si>
+  <si>
+    <t>Spanish (United States)</t>
+  </si>
+  <si>
+    <t>id-ID</t>
+  </si>
+  <si>
+    <t>Indonesian (Indonesia)</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Esperanto</t>
   </si>
 </sst>
 </file>
@@ -360,11 +558,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,9 +878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76702F4A-6822-104D-A228-EE608917D6A9}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -697,381 +898,646 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="A7" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
+      <c r="A11" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>37</v>
+      <c r="A12" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>46</v>
+      <c r="A14" t="s">
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
+      <c r="A17" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>6</v>
+      <c r="A20" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>9</v>
+      <c r="A23" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>10</v>
+      <c r="A24" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>11</v>
+      <c r="A29" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>36</v>
+      <c r="A30" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>13</v>
+      <c r="A33" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>14</v>
+      <c r="A34" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>15</v>
+      <c r="A36" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>16</v>
+      <c r="A37" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>18</v>
+      <c r="A39" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>63</v>
+      <c r="A40" t="s">
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>51</v>
+      <c r="A42" t="s">
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>66</v>
+      <c r="A44" t="s">
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B78" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>19</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B46" xr:uid="{309F8E5E-ED38-B949-88CE-AFA268C169D7}"/>
-  <sortState ref="A2:B46">
-    <sortCondition ref="A2:A46"/>
+  <autoFilter ref="A1:B79" xr:uid="{309F8E5E-ED38-B949-88CE-AFA268C169D7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B79">
+      <sortCondition ref="A4:A79"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B55">
+    <sortCondition ref="A4:A55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>